<commit_message>
Finished Sorting process, started on data entry in nhmrc
</commit_message>
<xml_diff>
--- a/Processes/RMS_HREAFormDataExtraction/Data/Config.xlsx
+++ b/Processes/RMS_HREAFormDataExtraction/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="5775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="5775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -216,10 +216,10 @@
     <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\DEV\RMS_HREAFormDataExtraction\Remaining</t>
   </si>
   <si>
-    <t>C:\UiPath\RpaUiPathProcess\Processes\RMS_HREAFormDataExtraction\Data\HREA ID linked to RM ID.xlsx</t>
-  </si>
-  <si>
     <t>LinkingWorkbook</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\DEV\RMS_HREAFormDataExtraction\HREA ID linked to RM ID.xlsx</t>
   </si>
 </sst>
 </file>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -615,14 +615,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1623,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1720,14 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Process_GatherAndCheck: Added middle stage to check that all files are present and compatible with an upload (nothing over 10MB, whole package under 95MB and all files exist) DataEntry workflows: Added throwing the inner exception from the retry scope so errors can actually be seen rather than the stupid "activity did not perform as expected" Moved the writing of temp files out of DEV mode only and set a folder on the network share called Bot Files. Consent: Needed to check the value of Q1.19 and Q2.2.P1.P3.1 DataAndPrivacy: Added handling of unassigned value for Q3.6.1
</commit_message>
<xml_diff>
--- a/Processes/RMS_HREAFormDataExtraction/Data/Config.xlsx
+++ b/Processes/RMS_HREAFormDataExtraction/Data/Config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\DEV\RMS_HREAFormDataExtraction\HREA ID linked to RM ID.xlsx</t>
+  </si>
+  <si>
+    <t>FileServer_BotFiles</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\DEV\RMS_HREAFormDataExtraction\Bot Files</t>
   </si>
 </sst>
 </file>
@@ -1614,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,16 +1725,25 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2712,6 +2727,7 @@
     <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commit of Test files and files with updated annotations only
</commit_message>
<xml_diff>
--- a/Processes/RMS_HREAFormDataExtraction/Data/Config.xlsx
+++ b/Processes/RMS_HREAFormDataExtraction/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\RpaUiPathProcess\Processes\RMS_HREAFormDataExtraction\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\RMS_HREAFormDataExtraction\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1127FDED-4D5E-49F8-A93E-763E15ACC7FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="5775" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -226,13 +227,28 @@
   </si>
   <si>
     <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\DEV\RMS_HREAFormDataExtraction\Bot Files</t>
+  </si>
+  <si>
+    <t>RMS_HREAMigration_PortalLogin</t>
+  </si>
+  <si>
+    <t>HREA Portal Login</t>
+  </si>
+  <si>
+    <t>SSO_rpa00004</t>
+  </si>
+  <si>
+    <t>https://uqomnistar2uat.f1solutions.com.au/</t>
+  </si>
+  <si>
+    <t>HREA Portal URL DEV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -243,6 +259,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -265,10 +287,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,11 +572,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -621,7 +645,14 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1615,15 +1646,16 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,7 +1710,7 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -2734,7 +2766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0"/>
@@ -3946,11 +3978,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4001,8 +4033,22 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>